<commit_message>
formatting updates, feel free to poke through and edit away! (deleted the duplicate docx file)
</commit_message>
<xml_diff>
--- a/timeTable.xlsx
+++ b/timeTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kurt Slagle\Documents\EECS-448-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a388p434\Dropbox\Gehrig\Programming\Qt\PasswordsGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -580,28 +580,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" customWidth="1"/>
-    <col min="4" max="4" width="5.875" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="5.125" customWidth="1"/>
-    <col min="7" max="7" width="5.375" customWidth="1"/>
-    <col min="8" max="8" width="6.25" customWidth="1"/>
-    <col min="9" max="9" width="6.375" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="6.25" customWidth="1"/>
-    <col min="13" max="13" width="6.5" customWidth="1"/>
-    <col min="14" max="14" width="6.375" customWidth="1"/>
-    <col min="15" max="15" width="8" customWidth="1"/>
+    <col min="2" max="15" width="3.625" customWidth="1"/>
     <col min="16" max="16" width="20.125" customWidth="1"/>
     <col min="17" max="19" width="4.625" customWidth="1"/>
   </cols>
@@ -613,12 +601,8 @@
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13">
-        <v>42129</v>
-      </c>
-      <c r="J1" s="13">
-        <v>42130</v>
-      </c>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="P1" t="s">
         <v>8</v>
       </c>
@@ -830,29 +814,23 @@
       <c r="A11" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>